<commit_message>
Getting to know the code
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1227,8 +1227,8 @@
   </x:sheetData>
   <x:phoneticPr fontId="2"/>
   <x:hyperlinks>
-    <x:hyperlink ref="B6" r:id="rId8"/>
-    <x:hyperlink ref="B9" r:id="rId9"/>
+    <x:hyperlink ref="B6" r:id="rId10"/>
+    <x:hyperlink ref="B9" r:id="rId11"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1915,8 +1915,8 @@
   </x:sheetData>
   <x:phoneticPr fontId="2"/>
   <x:hyperlinks>
-    <x:hyperlink ref="B10" r:id="rId14"/>
-    <x:hyperlink ref="B11" r:id="rId15"/>
+    <x:hyperlink ref="B10" r:id="rId12"/>
+    <x:hyperlink ref="B11" r:id="rId13"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>